<commit_message>
Added Shadow API. Added VIs to create policies for sending IoT data to S3, SNS, and SQS.
</commit_message>
<xml_diff>
--- a/source/_docs/Error Codes - AWS Toolkit - SQS.xlsx
+++ b/source/_docs/Error Codes - AWS Toolkit - SQS.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Code</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>The AWS SQS VIs do not currently support FIFO Queues.</t>
+  </si>
+  <si>
+    <t>The ARN for the specified SQS queue could not be found.</t>
   </si>
 </sst>
 </file>
@@ -441,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,6 +560,14 @@
         <v>13</v>
       </c>
     </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>412112</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>